<commit_message>
Ajout de l'ID de porte dans le formulaire de porte et validation requise
</commit_message>
<xml_diff>
--- a/documentation/3_2_Modele_PlanningLundiMardi.xlsx
+++ b/documentation/3_2_Modele_PlanningLundiMardi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\306-bersier\projet-306-tercier-morales-bersier\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eloua\Documents\projet-306-tercier-morales-bersier\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF1BE85-9E06-48A7-B8B1-D8B9EE814E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05747F-F3B8-4ED8-A122-591C88C662CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="62">
   <si>
     <t>Tous</t>
   </si>
@@ -1076,7 +1076,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1279,6 +1279,50 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1331,55 +1375,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1864,29 +1861,29 @@
   <dimension ref="A1:CF45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="AU9" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="BP36" sqref="BP36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" style="3" customWidth="1"/>
-    <col min="4" max="83" width="2.140625" style="2" customWidth="1"/>
-    <col min="84" max="84" width="3.140625" style="3" customWidth="1"/>
-    <col min="85" max="297" width="9.140625" style="3" customWidth="1"/>
-    <col min="298" max="16384" width="11.5703125" style="3"/>
+    <col min="1" max="1" width="66.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="3" customWidth="1"/>
+    <col min="4" max="83" width="2.1796875" style="2" customWidth="1"/>
+    <col min="84" max="84" width="3.1796875" style="3" customWidth="1"/>
+    <col min="85" max="297" width="9.1796875" style="3" customWidth="1"/>
+    <col min="298" max="16384" width="11.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:84" ht="23" x14ac:dyDescent="0.5">
+      <c r="A1" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
       <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1930,12 +1927,12 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:84" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:84" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1977,7 +1974,7 @@
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="1:84" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:84" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
@@ -2024,12 +2021,12 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2076,184 +2073,184 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:84" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:84" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="77">
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="66">
         <v>0</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="77"/>
-      <c r="T5" s="77"/>
-      <c r="U5" s="77"/>
-      <c r="V5" s="77"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="77"/>
-      <c r="Y5" s="77"/>
-      <c r="Z5" s="77"/>
-      <c r="AA5" s="77"/>
-      <c r="AB5" s="77"/>
-      <c r="AC5" s="77"/>
-      <c r="AD5" s="77"/>
-      <c r="AE5" s="77"/>
-      <c r="AF5" s="77"/>
-      <c r="AG5" s="77"/>
-      <c r="AH5" s="77"/>
-      <c r="AI5" s="77"/>
-      <c r="AJ5" s="77"/>
-      <c r="AK5" s="77"/>
-      <c r="AL5" s="77"/>
-      <c r="AM5" s="77"/>
-      <c r="AN5" s="77"/>
-      <c r="AO5" s="77"/>
-      <c r="AP5" s="77"/>
-      <c r="AQ5" s="77"/>
-      <c r="AR5" s="77"/>
-      <c r="AS5" s="77"/>
-      <c r="AT5" s="77"/>
-      <c r="AU5" s="77"/>
-      <c r="AV5" s="77"/>
-      <c r="AW5" s="77"/>
-      <c r="AX5" s="77"/>
-      <c r="AY5" s="77"/>
-      <c r="AZ5" s="77"/>
-      <c r="BA5" s="77"/>
-      <c r="BB5" s="77"/>
-      <c r="BC5" s="77"/>
-      <c r="BD5" s="77"/>
-      <c r="BE5" s="77"/>
-      <c r="BF5" s="77"/>
-      <c r="BG5" s="77"/>
-      <c r="BH5" s="77"/>
-      <c r="BI5" s="77"/>
-      <c r="BJ5" s="77"/>
-      <c r="BK5" s="77"/>
-      <c r="BL5" s="77"/>
-      <c r="BM5" s="77"/>
-      <c r="BN5" s="77"/>
-      <c r="BO5" s="77"/>
-      <c r="BP5" s="77"/>
-      <c r="BQ5" s="77"/>
-      <c r="BR5" s="77"/>
-      <c r="BS5" s="77"/>
-      <c r="BT5" s="77"/>
-      <c r="BU5" s="77"/>
-      <c r="BV5" s="77"/>
-      <c r="BW5" s="77"/>
-      <c r="BX5" s="77"/>
-      <c r="BY5" s="77"/>
-      <c r="BZ5" s="77"/>
-      <c r="CA5" s="77"/>
-      <c r="CB5" s="77"/>
-      <c r="CC5" s="77"/>
-      <c r="CD5" s="77"/>
-      <c r="CE5" s="77"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
+      <c r="Y5" s="66"/>
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="66"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="66"/>
+      <c r="AD5" s="66"/>
+      <c r="AE5" s="66"/>
+      <c r="AF5" s="66"/>
+      <c r="AG5" s="66"/>
+      <c r="AH5" s="66"/>
+      <c r="AI5" s="66"/>
+      <c r="AJ5" s="66"/>
+      <c r="AK5" s="66"/>
+      <c r="AL5" s="66"/>
+      <c r="AM5" s="66"/>
+      <c r="AN5" s="66"/>
+      <c r="AO5" s="66"/>
+      <c r="AP5" s="66"/>
+      <c r="AQ5" s="66"/>
+      <c r="AR5" s="66"/>
+      <c r="AS5" s="66"/>
+      <c r="AT5" s="66"/>
+      <c r="AU5" s="66"/>
+      <c r="AV5" s="66"/>
+      <c r="AW5" s="66"/>
+      <c r="AX5" s="66"/>
+      <c r="AY5" s="66"/>
+      <c r="AZ5" s="66"/>
+      <c r="BA5" s="66"/>
+      <c r="BB5" s="66"/>
+      <c r="BC5" s="66"/>
+      <c r="BD5" s="66"/>
+      <c r="BE5" s="66"/>
+      <c r="BF5" s="66"/>
+      <c r="BG5" s="66"/>
+      <c r="BH5" s="66"/>
+      <c r="BI5" s="66"/>
+      <c r="BJ5" s="66"/>
+      <c r="BK5" s="66"/>
+      <c r="BL5" s="66"/>
+      <c r="BM5" s="66"/>
+      <c r="BN5" s="66"/>
+      <c r="BO5" s="66"/>
+      <c r="BP5" s="66"/>
+      <c r="BQ5" s="66"/>
+      <c r="BR5" s="66"/>
+      <c r="BS5" s="66"/>
+      <c r="BT5" s="66"/>
+      <c r="BU5" s="66"/>
+      <c r="BV5" s="66"/>
+      <c r="BW5" s="66"/>
+      <c r="BX5" s="66"/>
+      <c r="BY5" s="66"/>
+      <c r="BZ5" s="66"/>
+      <c r="CA5" s="66"/>
+      <c r="CB5" s="66"/>
+      <c r="CC5" s="66"/>
+      <c r="CD5" s="66"/>
+      <c r="CE5" s="66"/>
     </row>
-    <row r="6" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="78"/>
-      <c r="AB6" s="78"/>
-      <c r="AC6" s="78"/>
-      <c r="AD6" s="78"/>
-      <c r="AE6" s="78"/>
-      <c r="AF6" s="78"/>
-      <c r="AG6" s="78"/>
-      <c r="AH6" s="78"/>
-      <c r="AI6" s="78"/>
-      <c r="AJ6" s="78"/>
-      <c r="AK6" s="78"/>
-      <c r="AL6" s="78"/>
-      <c r="AM6" s="78"/>
-      <c r="AN6" s="78"/>
-      <c r="AO6" s="78"/>
-      <c r="AP6" s="78"/>
-      <c r="AQ6" s="78"/>
-      <c r="AR6" s="78"/>
-      <c r="AS6" s="78"/>
-      <c r="AT6" s="78"/>
-      <c r="AU6" s="78"/>
-      <c r="AV6" s="78"/>
-      <c r="AW6" s="78"/>
-      <c r="AX6" s="78"/>
-      <c r="AY6" s="78"/>
-      <c r="AZ6" s="78"/>
-      <c r="BA6" s="78"/>
-      <c r="BB6" s="78"/>
-      <c r="BC6" s="78"/>
-      <c r="BD6" s="78"/>
-      <c r="BE6" s="78"/>
-      <c r="BF6" s="78"/>
-      <c r="BG6" s="78"/>
-      <c r="BH6" s="78"/>
-      <c r="BI6" s="78"/>
-      <c r="BJ6" s="78"/>
-      <c r="BK6" s="78"/>
-      <c r="BL6" s="78"/>
-      <c r="BM6" s="78"/>
-      <c r="BN6" s="78"/>
-      <c r="BO6" s="78"/>
-      <c r="BP6" s="78"/>
-      <c r="BQ6" s="78"/>
-      <c r="BR6" s="78"/>
-      <c r="BS6" s="78"/>
-      <c r="BT6" s="78"/>
-      <c r="BU6" s="78"/>
-      <c r="BV6" s="78"/>
-      <c r="BW6" s="78"/>
-      <c r="BX6" s="78"/>
-      <c r="BY6" s="78"/>
-      <c r="BZ6" s="78"/>
-      <c r="CA6" s="78"/>
-      <c r="CB6" s="78"/>
-      <c r="CC6" s="78"/>
-      <c r="CD6" s="78"/>
-      <c r="CE6" s="78"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="67"/>
+      <c r="Y6" s="67"/>
+      <c r="Z6" s="67"/>
+      <c r="AA6" s="67"/>
+      <c r="AB6" s="67"/>
+      <c r="AC6" s="67"/>
+      <c r="AD6" s="67"/>
+      <c r="AE6" s="67"/>
+      <c r="AF6" s="67"/>
+      <c r="AG6" s="67"/>
+      <c r="AH6" s="67"/>
+      <c r="AI6" s="67"/>
+      <c r="AJ6" s="67"/>
+      <c r="AK6" s="67"/>
+      <c r="AL6" s="67"/>
+      <c r="AM6" s="67"/>
+      <c r="AN6" s="67"/>
+      <c r="AO6" s="67"/>
+      <c r="AP6" s="67"/>
+      <c r="AQ6" s="67"/>
+      <c r="AR6" s="67"/>
+      <c r="AS6" s="67"/>
+      <c r="AT6" s="67"/>
+      <c r="AU6" s="67"/>
+      <c r="AV6" s="67"/>
+      <c r="AW6" s="67"/>
+      <c r="AX6" s="67"/>
+      <c r="AY6" s="67"/>
+      <c r="AZ6" s="67"/>
+      <c r="BA6" s="67"/>
+      <c r="BB6" s="67"/>
+      <c r="BC6" s="67"/>
+      <c r="BD6" s="67"/>
+      <c r="BE6" s="67"/>
+      <c r="BF6" s="67"/>
+      <c r="BG6" s="67"/>
+      <c r="BH6" s="67"/>
+      <c r="BI6" s="67"/>
+      <c r="BJ6" s="67"/>
+      <c r="BK6" s="67"/>
+      <c r="BL6" s="67"/>
+      <c r="BM6" s="67"/>
+      <c r="BN6" s="67"/>
+      <c r="BO6" s="67"/>
+      <c r="BP6" s="67"/>
+      <c r="BQ6" s="67"/>
+      <c r="BR6" s="67"/>
+      <c r="BS6" s="67"/>
+      <c r="BT6" s="67"/>
+      <c r="BU6" s="67"/>
+      <c r="BV6" s="67"/>
+      <c r="BW6" s="67"/>
+      <c r="BX6" s="67"/>
+      <c r="BY6" s="67"/>
+      <c r="BZ6" s="67"/>
+      <c r="CA6" s="67"/>
+      <c r="CB6" s="67"/>
+      <c r="CC6" s="67"/>
+      <c r="CD6" s="67"/>
+      <c r="CE6" s="67"/>
     </row>
-    <row r="7" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61" t="s">
+    <row r="7" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="72" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="18" t="s">
@@ -2262,132 +2259,132 @@
       <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74">
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="62">
         <v>45992</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="72" t="s">
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="74">
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="62">
         <v>45993</v>
       </c>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="75"/>
-      <c r="T7" s="72" t="s">
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="73"/>
-      <c r="V7" s="73"/>
-      <c r="W7" s="73"/>
-      <c r="X7" s="74">
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="62">
         <v>45999</v>
       </c>
-      <c r="Y7" s="74"/>
-      <c r="Z7" s="74"/>
-      <c r="AA7" s="75"/>
-      <c r="AB7" s="72" t="s">
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="63"/>
+      <c r="AB7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="AC7" s="73"/>
-      <c r="AD7" s="73"/>
-      <c r="AE7" s="73"/>
-      <c r="AF7" s="74">
+      <c r="AC7" s="65"/>
+      <c r="AD7" s="65"/>
+      <c r="AE7" s="65"/>
+      <c r="AF7" s="62">
         <v>46000</v>
       </c>
-      <c r="AG7" s="74"/>
-      <c r="AH7" s="74"/>
-      <c r="AI7" s="75"/>
-      <c r="AJ7" s="72" t="s">
+      <c r="AG7" s="62"/>
+      <c r="AH7" s="62"/>
+      <c r="AI7" s="63"/>
+      <c r="AJ7" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="AK7" s="73"/>
-      <c r="AL7" s="73"/>
-      <c r="AM7" s="73"/>
-      <c r="AN7" s="74">
+      <c r="AK7" s="65"/>
+      <c r="AL7" s="65"/>
+      <c r="AM7" s="65"/>
+      <c r="AN7" s="62">
         <v>46006</v>
       </c>
-      <c r="AO7" s="74"/>
-      <c r="AP7" s="74"/>
-      <c r="AQ7" s="75"/>
-      <c r="AR7" s="72" t="s">
+      <c r="AO7" s="62"/>
+      <c r="AP7" s="62"/>
+      <c r="AQ7" s="63"/>
+      <c r="AR7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="AS7" s="73"/>
-      <c r="AT7" s="73"/>
-      <c r="AU7" s="73"/>
-      <c r="AV7" s="74">
+      <c r="AS7" s="65"/>
+      <c r="AT7" s="65"/>
+      <c r="AU7" s="65"/>
+      <c r="AV7" s="62">
         <v>46007</v>
       </c>
-      <c r="AW7" s="74"/>
-      <c r="AX7" s="74"/>
-      <c r="AY7" s="75"/>
-      <c r="AZ7" s="72" t="s">
+      <c r="AW7" s="62"/>
+      <c r="AX7" s="62"/>
+      <c r="AY7" s="63"/>
+      <c r="AZ7" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="BA7" s="73"/>
-      <c r="BB7" s="73"/>
-      <c r="BC7" s="73"/>
-      <c r="BD7" s="74">
+      <c r="BA7" s="65"/>
+      <c r="BB7" s="65"/>
+      <c r="BC7" s="65"/>
+      <c r="BD7" s="62">
         <v>46027</v>
       </c>
-      <c r="BE7" s="74"/>
-      <c r="BF7" s="74"/>
-      <c r="BG7" s="75"/>
-      <c r="BH7" s="72" t="s">
+      <c r="BE7" s="62"/>
+      <c r="BF7" s="62"/>
+      <c r="BG7" s="63"/>
+      <c r="BH7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="BI7" s="73"/>
-      <c r="BJ7" s="73"/>
-      <c r="BK7" s="73"/>
-      <c r="BL7" s="74">
+      <c r="BI7" s="65"/>
+      <c r="BJ7" s="65"/>
+      <c r="BK7" s="65"/>
+      <c r="BL7" s="62">
         <v>46028</v>
       </c>
-      <c r="BM7" s="74"/>
-      <c r="BN7" s="74"/>
-      <c r="BO7" s="75"/>
-      <c r="BP7" s="72" t="s">
+      <c r="BM7" s="62"/>
+      <c r="BN7" s="62"/>
+      <c r="BO7" s="63"/>
+      <c r="BP7" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="BQ7" s="73"/>
-      <c r="BR7" s="73"/>
-      <c r="BS7" s="73"/>
-      <c r="BT7" s="74">
+      <c r="BQ7" s="65"/>
+      <c r="BR7" s="65"/>
+      <c r="BS7" s="65"/>
+      <c r="BT7" s="62">
         <v>46034</v>
       </c>
-      <c r="BU7" s="74"/>
-      <c r="BV7" s="74"/>
-      <c r="BW7" s="75"/>
-      <c r="BX7" s="72" t="s">
+      <c r="BU7" s="62"/>
+      <c r="BV7" s="62"/>
+      <c r="BW7" s="63"/>
+      <c r="BX7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="BY7" s="73"/>
-      <c r="BZ7" s="73"/>
-      <c r="CA7" s="73"/>
-      <c r="CB7" s="74">
+      <c r="BY7" s="65"/>
+      <c r="BZ7" s="65"/>
+      <c r="CA7" s="65"/>
+      <c r="CB7" s="62">
         <v>46035</v>
       </c>
-      <c r="CC7" s="74"/>
-      <c r="CD7" s="74"/>
-      <c r="CE7" s="75"/>
-      <c r="CF7" s="60" t="s">
+      <c r="CC7" s="62"/>
+      <c r="CD7" s="62"/>
+      <c r="CE7" s="63"/>
+      <c r="CF7" s="71" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
+    <row r="8" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="73"/>
       <c r="B8" s="19" t="s">
         <v>11</v>
       </c>
@@ -2634,9 +2631,9 @@
       <c r="CE8" s="7">
         <v>8</v>
       </c>
-      <c r="CF8" s="60"/>
+      <c r="CF8" s="71"/>
     </row>
-    <row r="9" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="35" t="s">
         <v>17</v>
       </c>
@@ -2644,10 +2641,10 @@
         <v>29</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
       <c r="H9" s="44"/>
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
@@ -2660,16 +2657,16 @@
       <c r="Q9" s="44"/>
       <c r="R9" s="44"/>
       <c r="S9" s="44"/>
-      <c r="T9" s="63" t="s">
+      <c r="T9" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="65"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+      <c r="X9" s="75"/>
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="75"/>
+      <c r="AA9" s="76"/>
       <c r="AB9" s="44"/>
       <c r="AC9" s="44"/>
       <c r="AD9" s="44"/>
@@ -2726,9 +2723,9 @@
       <c r="CC9" s="44"/>
       <c r="CD9" s="44"/>
       <c r="CE9" s="44"/>
-      <c r="CF9" s="60"/>
+      <c r="CF9" s="71"/>
     </row>
-    <row r="10" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="36" t="s">
         <v>18</v>
       </c>
@@ -2740,10 +2737,10 @@
       <c r="E10" s="44"/>
       <c r="F10" s="44"/>
       <c r="G10" s="44"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
       <c r="L10" s="44"/>
       <c r="M10" s="44"/>
       <c r="N10" s="44"/>
@@ -2752,14 +2749,14 @@
       <c r="Q10" s="44"/>
       <c r="R10" s="44"/>
       <c r="S10" s="44"/>
-      <c r="T10" s="66"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="67"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="68"/>
+      <c r="T10" s="77"/>
+      <c r="U10" s="78"/>
+      <c r="V10" s="78"/>
+      <c r="W10" s="78"/>
+      <c r="X10" s="78"/>
+      <c r="Y10" s="78"/>
+      <c r="Z10" s="78"/>
+      <c r="AA10" s="79"/>
       <c r="AB10" s="44"/>
       <c r="AC10" s="44"/>
       <c r="AD10" s="44"/>
@@ -2816,9 +2813,9 @@
       <c r="CC10" s="44"/>
       <c r="CD10" s="44"/>
       <c r="CE10" s="44"/>
-      <c r="CF10" s="60"/>
+      <c r="CF10" s="71"/>
     </row>
-    <row r="11" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>19</v>
       </c>
@@ -2842,14 +2839,14 @@
       <c r="Q11" s="44"/>
       <c r="R11" s="44"/>
       <c r="S11" s="44"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="67"/>
-      <c r="W11" s="67"/>
-      <c r="X11" s="67"/>
-      <c r="Y11" s="67"/>
-      <c r="Z11" s="67"/>
-      <c r="AA11" s="68"/>
+      <c r="T11" s="77"/>
+      <c r="U11" s="78"/>
+      <c r="V11" s="78"/>
+      <c r="W11" s="78"/>
+      <c r="X11" s="78"/>
+      <c r="Y11" s="78"/>
+      <c r="Z11" s="78"/>
+      <c r="AA11" s="79"/>
       <c r="AB11" s="44"/>
       <c r="AC11" s="44"/>
       <c r="AD11" s="44"/>
@@ -2906,9 +2903,9 @@
       <c r="CC11" s="44"/>
       <c r="CD11" s="44"/>
       <c r="CE11" s="44"/>
-      <c r="CF11" s="60"/>
+      <c r="CF11" s="71"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>20</v>
       </c>
@@ -2932,14 +2929,14 @@
       <c r="Q12" s="44"/>
       <c r="R12" s="44"/>
       <c r="S12" s="44"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="67"/>
-      <c r="V12" s="67"/>
-      <c r="W12" s="67"/>
-      <c r="X12" s="67"/>
-      <c r="Y12" s="67"/>
-      <c r="Z12" s="67"/>
-      <c r="AA12" s="68"/>
+      <c r="T12" s="77"/>
+      <c r="U12" s="78"/>
+      <c r="V12" s="78"/>
+      <c r="W12" s="78"/>
+      <c r="X12" s="78"/>
+      <c r="Y12" s="78"/>
+      <c r="Z12" s="78"/>
+      <c r="AA12" s="79"/>
       <c r="AB12" s="44"/>
       <c r="AC12" s="44"/>
       <c r="AD12" s="44"/>
@@ -2996,9 +2993,9 @@
       <c r="CC12" s="44"/>
       <c r="CD12" s="44"/>
       <c r="CE12" s="44"/>
-      <c r="CF12" s="60"/>
+      <c r="CF12" s="71"/>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="58" t="s">
         <v>42</v>
       </c>
@@ -3022,14 +3019,14 @@
       <c r="Q13" s="44"/>
       <c r="R13" s="44"/>
       <c r="S13" s="44"/>
-      <c r="T13" s="66"/>
-      <c r="U13" s="67"/>
-      <c r="V13" s="67"/>
-      <c r="W13" s="67"/>
-      <c r="X13" s="67"/>
-      <c r="Y13" s="67"/>
-      <c r="Z13" s="67"/>
-      <c r="AA13" s="68"/>
+      <c r="T13" s="77"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="78"/>
+      <c r="W13" s="78"/>
+      <c r="X13" s="78"/>
+      <c r="Y13" s="78"/>
+      <c r="Z13" s="78"/>
+      <c r="AA13" s="79"/>
       <c r="AB13" s="44"/>
       <c r="AC13" s="44"/>
       <c r="AD13" s="44"/>
@@ -3086,9 +3083,9 @@
       <c r="CC13" s="44"/>
       <c r="CD13" s="44"/>
       <c r="CE13" s="44"/>
-      <c r="CF13" s="60"/>
+      <c r="CF13" s="71"/>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="58" t="s">
         <v>43</v>
       </c>
@@ -3112,14 +3109,14 @@
       <c r="Q14" s="44"/>
       <c r="R14" s="44"/>
       <c r="S14" s="44"/>
-      <c r="T14" s="66"/>
-      <c r="U14" s="67"/>
-      <c r="V14" s="67"/>
-      <c r="W14" s="67"/>
-      <c r="X14" s="67"/>
-      <c r="Y14" s="67"/>
-      <c r="Z14" s="67"/>
-      <c r="AA14" s="68"/>
+      <c r="T14" s="77"/>
+      <c r="U14" s="78"/>
+      <c r="V14" s="78"/>
+      <c r="W14" s="78"/>
+      <c r="X14" s="78"/>
+      <c r="Y14" s="78"/>
+      <c r="Z14" s="78"/>
+      <c r="AA14" s="79"/>
       <c r="AB14" s="45" t="s">
         <v>39</v>
       </c>
@@ -3178,9 +3175,9 @@
       <c r="CC14" s="44"/>
       <c r="CD14" s="44"/>
       <c r="CE14" s="44"/>
-      <c r="CF14" s="60"/>
+      <c r="CF14" s="71"/>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="58" t="s">
         <v>44</v>
       </c>
@@ -3204,14 +3201,14 @@
       <c r="Q15" s="44"/>
       <c r="R15" s="44"/>
       <c r="S15" s="44"/>
-      <c r="T15" s="66"/>
-      <c r="U15" s="67"/>
-      <c r="V15" s="67"/>
-      <c r="W15" s="67"/>
-      <c r="X15" s="67"/>
-      <c r="Y15" s="67"/>
-      <c r="Z15" s="67"/>
-      <c r="AA15" s="68"/>
+      <c r="T15" s="77"/>
+      <c r="U15" s="78"/>
+      <c r="V15" s="78"/>
+      <c r="W15" s="78"/>
+      <c r="X15" s="78"/>
+      <c r="Y15" s="78"/>
+      <c r="Z15" s="78"/>
+      <c r="AA15" s="79"/>
       <c r="AB15" s="44"/>
       <c r="AC15" s="45" t="s">
         <v>39</v>
@@ -3278,9 +3275,9 @@
       <c r="CC15" s="44"/>
       <c r="CD15" s="44"/>
       <c r="CE15" s="44"/>
-      <c r="CF15" s="60"/>
+      <c r="CF15" s="71"/>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>34</v>
       </c>
@@ -3302,14 +3299,14 @@
       <c r="Q16" s="44"/>
       <c r="R16" s="44"/>
       <c r="S16" s="44"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="67"/>
-      <c r="V16" s="67"/>
-      <c r="W16" s="67"/>
-      <c r="X16" s="67"/>
-      <c r="Y16" s="67"/>
-      <c r="Z16" s="67"/>
-      <c r="AA16" s="68"/>
+      <c r="T16" s="77"/>
+      <c r="U16" s="78"/>
+      <c r="V16" s="78"/>
+      <c r="W16" s="78"/>
+      <c r="X16" s="78"/>
+      <c r="Y16" s="78"/>
+      <c r="Z16" s="78"/>
+      <c r="AA16" s="79"/>
       <c r="AB16" s="44"/>
       <c r="AC16" s="44"/>
       <c r="AD16" s="44"/>
@@ -3366,9 +3363,9 @@
       <c r="CC16" s="44"/>
       <c r="CD16" s="44"/>
       <c r="CE16" s="44"/>
-      <c r="CF16" s="60"/>
+      <c r="CF16" s="71"/>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>45</v>
       </c>
@@ -3390,14 +3387,14 @@
       <c r="Q17" s="44"/>
       <c r="R17" s="44"/>
       <c r="S17" s="44"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="67"/>
-      <c r="V17" s="67"/>
-      <c r="W17" s="67"/>
-      <c r="X17" s="67"/>
-      <c r="Y17" s="67"/>
-      <c r="Z17" s="67"/>
-      <c r="AA17" s="68"/>
+      <c r="T17" s="77"/>
+      <c r="U17" s="78"/>
+      <c r="V17" s="78"/>
+      <c r="W17" s="78"/>
+      <c r="X17" s="78"/>
+      <c r="Y17" s="78"/>
+      <c r="Z17" s="78"/>
+      <c r="AA17" s="79"/>
       <c r="AB17" s="44"/>
       <c r="AC17" s="44"/>
       <c r="AD17" s="44"/>
@@ -3464,9 +3461,9 @@
       <c r="CC17" s="44"/>
       <c r="CD17" s="44"/>
       <c r="CE17" s="44"/>
-      <c r="CF17" s="60"/>
+      <c r="CF17" s="71"/>
     </row>
-    <row r="18" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
         <v>46</v>
       </c>
@@ -3488,14 +3485,14 @@
       <c r="Q18" s="44"/>
       <c r="R18" s="44"/>
       <c r="S18" s="44"/>
-      <c r="T18" s="66"/>
-      <c r="U18" s="67"/>
-      <c r="V18" s="67"/>
-      <c r="W18" s="67"/>
-      <c r="X18" s="67"/>
-      <c r="Y18" s="67"/>
-      <c r="Z18" s="67"/>
-      <c r="AA18" s="68"/>
+      <c r="T18" s="77"/>
+      <c r="U18" s="78"/>
+      <c r="V18" s="78"/>
+      <c r="W18" s="78"/>
+      <c r="X18" s="78"/>
+      <c r="Y18" s="78"/>
+      <c r="Z18" s="78"/>
+      <c r="AA18" s="79"/>
       <c r="AB18" s="44"/>
       <c r="AC18" s="44"/>
       <c r="AD18" s="44"/>
@@ -3558,9 +3555,9 @@
       <c r="CC18" s="44"/>
       <c r="CD18" s="44"/>
       <c r="CE18" s="44"/>
-      <c r="CF18" s="60"/>
+      <c r="CF18" s="71"/>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>47</v>
       </c>
@@ -3582,14 +3579,14 @@
       <c r="Q19" s="44"/>
       <c r="R19" s="44"/>
       <c r="S19" s="44"/>
-      <c r="T19" s="66"/>
-      <c r="U19" s="67"/>
-      <c r="V19" s="67"/>
-      <c r="W19" s="67"/>
-      <c r="X19" s="67"/>
-      <c r="Y19" s="67"/>
-      <c r="Z19" s="67"/>
-      <c r="AA19" s="68"/>
+      <c r="T19" s="77"/>
+      <c r="U19" s="78"/>
+      <c r="V19" s="78"/>
+      <c r="W19" s="78"/>
+      <c r="X19" s="78"/>
+      <c r="Y19" s="78"/>
+      <c r="Z19" s="78"/>
+      <c r="AA19" s="79"/>
       <c r="AB19" s="44"/>
       <c r="AC19" s="44"/>
       <c r="AD19" s="44"/>
@@ -3654,9 +3651,9 @@
       <c r="CC19" s="44"/>
       <c r="CD19" s="44"/>
       <c r="CE19" s="44"/>
-      <c r="CF19" s="60"/>
+      <c r="CF19" s="71"/>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>59</v>
       </c>
@@ -3678,14 +3675,14 @@
       <c r="Q20" s="44"/>
       <c r="R20" s="44"/>
       <c r="S20" s="44"/>
-      <c r="T20" s="66"/>
-      <c r="U20" s="67"/>
-      <c r="V20" s="67"/>
-      <c r="W20" s="67"/>
-      <c r="X20" s="67"/>
-      <c r="Y20" s="67"/>
-      <c r="Z20" s="67"/>
-      <c r="AA20" s="68"/>
+      <c r="T20" s="77"/>
+      <c r="U20" s="78"/>
+      <c r="V20" s="78"/>
+      <c r="W20" s="78"/>
+      <c r="X20" s="78"/>
+      <c r="Y20" s="78"/>
+      <c r="Z20" s="78"/>
+      <c r="AA20" s="79"/>
       <c r="AB20" s="44"/>
       <c r="AC20" s="44"/>
       <c r="AD20" s="44"/>
@@ -3714,14 +3711,30 @@
       <c r="BA20" s="44"/>
       <c r="BB20" s="44"/>
       <c r="BC20" s="44"/>
-      <c r="BD20" s="49"/>
-      <c r="BE20" s="49"/>
-      <c r="BF20" s="49"/>
-      <c r="BG20" s="49"/>
-      <c r="BH20" s="44"/>
-      <c r="BI20" s="44"/>
-      <c r="BJ20" s="44"/>
-      <c r="BK20" s="44"/>
+      <c r="BD20" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="BE20" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF20" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG20" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="BH20" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BI20" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BJ20" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BK20" s="46" t="s">
+        <v>41</v>
+      </c>
       <c r="BL20" s="44"/>
       <c r="BM20" s="44"/>
       <c r="BN20" s="44"/>
@@ -3742,9 +3755,9 @@
       <c r="CC20" s="44"/>
       <c r="CD20" s="44"/>
       <c r="CE20" s="44"/>
-      <c r="CF20" s="60"/>
+      <c r="CF20" s="71"/>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>35</v>
       </c>
@@ -3766,14 +3779,14 @@
       <c r="Q21" s="44"/>
       <c r="R21" s="44"/>
       <c r="S21" s="44"/>
-      <c r="T21" s="66"/>
-      <c r="U21" s="67"/>
-      <c r="V21" s="67"/>
-      <c r="W21" s="67"/>
-      <c r="X21" s="67"/>
-      <c r="Y21" s="67"/>
-      <c r="Z21" s="67"/>
-      <c r="AA21" s="68"/>
+      <c r="T21" s="77"/>
+      <c r="U21" s="78"/>
+      <c r="V21" s="78"/>
+      <c r="W21" s="78"/>
+      <c r="X21" s="78"/>
+      <c r="Y21" s="78"/>
+      <c r="Z21" s="78"/>
+      <c r="AA21" s="79"/>
       <c r="AB21" s="44"/>
       <c r="AC21" s="44"/>
       <c r="AD21" s="44"/>
@@ -3806,10 +3819,6 @@
       <c r="BE21" s="44"/>
       <c r="BF21" s="44"/>
       <c r="BG21" s="44"/>
-      <c r="BH21" s="44"/>
-      <c r="BI21" s="44"/>
-      <c r="BJ21" s="44"/>
-      <c r="BK21" s="44"/>
       <c r="BL21" s="44"/>
       <c r="BM21" s="44"/>
       <c r="BN21" s="44"/>
@@ -3830,9 +3839,9 @@
       <c r="CC21" s="44"/>
       <c r="CD21" s="44"/>
       <c r="CE21" s="44"/>
-      <c r="CF21" s="60"/>
+      <c r="CF21" s="71"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>48</v>
       </c>
@@ -3854,14 +3863,14 @@
       <c r="Q22" s="44"/>
       <c r="R22" s="44"/>
       <c r="S22" s="44"/>
-      <c r="T22" s="66"/>
-      <c r="U22" s="67"/>
-      <c r="V22" s="67"/>
-      <c r="W22" s="67"/>
-      <c r="X22" s="67"/>
-      <c r="Y22" s="67"/>
-      <c r="Z22" s="67"/>
-      <c r="AA22" s="68"/>
+      <c r="T22" s="77"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="78"/>
+      <c r="W22" s="78"/>
+      <c r="X22" s="78"/>
+      <c r="Y22" s="78"/>
+      <c r="Z22" s="78"/>
+      <c r="AA22" s="79"/>
       <c r="AB22" s="44"/>
       <c r="AC22" s="44"/>
       <c r="AD22" s="44"/>
@@ -3922,9 +3931,9 @@
       <c r="CC22" s="44"/>
       <c r="CD22" s="44"/>
       <c r="CE22" s="44"/>
-      <c r="CF22" s="60"/>
+      <c r="CF22" s="71"/>
     </row>
-    <row r="23" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
         <v>49</v>
       </c>
@@ -3946,14 +3955,14 @@
       <c r="Q23" s="44"/>
       <c r="R23" s="44"/>
       <c r="S23" s="44"/>
-      <c r="T23" s="66"/>
-      <c r="U23" s="67"/>
-      <c r="V23" s="67"/>
-      <c r="W23" s="67"/>
-      <c r="X23" s="67"/>
-      <c r="Y23" s="67"/>
-      <c r="Z23" s="67"/>
-      <c r="AA23" s="68"/>
+      <c r="T23" s="77"/>
+      <c r="U23" s="78"/>
+      <c r="V23" s="78"/>
+      <c r="W23" s="78"/>
+      <c r="X23" s="78"/>
+      <c r="Y23" s="78"/>
+      <c r="Z23" s="78"/>
+      <c r="AA23" s="79"/>
       <c r="AB23" s="44"/>
       <c r="AC23" s="44"/>
       <c r="AD23" s="44"/>
@@ -4009,9 +4018,9 @@
       <c r="CC23" s="44"/>
       <c r="CD23" s="44"/>
       <c r="CE23" s="44"/>
-      <c r="CF23" s="60"/>
+      <c r="CF23" s="71"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>50</v>
       </c>
@@ -4033,14 +4042,14 @@
       <c r="Q24" s="44"/>
       <c r="R24" s="44"/>
       <c r="S24" s="44"/>
-      <c r="T24" s="66"/>
-      <c r="U24" s="67"/>
-      <c r="V24" s="67"/>
-      <c r="W24" s="67"/>
-      <c r="X24" s="67"/>
-      <c r="Y24" s="67"/>
-      <c r="Z24" s="67"/>
-      <c r="AA24" s="68"/>
+      <c r="T24" s="77"/>
+      <c r="U24" s="78"/>
+      <c r="V24" s="78"/>
+      <c r="W24" s="78"/>
+      <c r="X24" s="78"/>
+      <c r="Y24" s="78"/>
+      <c r="Z24" s="78"/>
+      <c r="AA24" s="79"/>
       <c r="AB24" s="44"/>
       <c r="AC24" s="44"/>
       <c r="AD24" s="44"/>
@@ -4097,9 +4106,9 @@
       <c r="CC24" s="44"/>
       <c r="CD24" s="44"/>
       <c r="CE24" s="44"/>
-      <c r="CF24" s="60"/>
+      <c r="CF24" s="71"/>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="36" t="s">
         <v>51</v>
       </c>
@@ -4121,14 +4130,14 @@
       <c r="Q25" s="44"/>
       <c r="R25" s="44"/>
       <c r="S25" s="44"/>
-      <c r="T25" s="66"/>
-      <c r="U25" s="67"/>
-      <c r="V25" s="67"/>
-      <c r="W25" s="67"/>
-      <c r="X25" s="67"/>
-      <c r="Y25" s="67"/>
-      <c r="Z25" s="67"/>
-      <c r="AA25" s="68"/>
+      <c r="T25" s="77"/>
+      <c r="U25" s="78"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="79"/>
       <c r="AB25" s="44"/>
       <c r="AC25" s="44"/>
       <c r="AD25" s="44"/>
@@ -4187,9 +4196,9 @@
       <c r="CC25" s="44"/>
       <c r="CD25" s="44"/>
       <c r="CE25" s="44"/>
-      <c r="CF25" s="60"/>
+      <c r="CF25" s="71"/>
     </row>
-    <row r="26" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="38" t="s">
         <v>52</v>
       </c>
@@ -4211,14 +4220,14 @@
       <c r="Q26" s="44"/>
       <c r="R26" s="44"/>
       <c r="S26" s="44"/>
-      <c r="T26" s="66"/>
-      <c r="U26" s="67"/>
-      <c r="V26" s="67"/>
-      <c r="W26" s="67"/>
-      <c r="X26" s="67"/>
-      <c r="Y26" s="67"/>
-      <c r="Z26" s="67"/>
-      <c r="AA26" s="68"/>
+      <c r="T26" s="77"/>
+      <c r="U26" s="78"/>
+      <c r="V26" s="78"/>
+      <c r="W26" s="78"/>
+      <c r="X26" s="78"/>
+      <c r="Y26" s="78"/>
+      <c r="Z26" s="78"/>
+      <c r="AA26" s="79"/>
       <c r="AB26" s="44"/>
       <c r="AC26" s="44"/>
       <c r="AD26" s="44"/>
@@ -4275,9 +4284,9 @@
       <c r="CC26" s="44"/>
       <c r="CD26" s="44"/>
       <c r="CE26" s="44"/>
-      <c r="CF26" s="60"/>
+      <c r="CF26" s="71"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
         <v>36</v>
       </c>
@@ -4299,14 +4308,14 @@
       <c r="Q27" s="44"/>
       <c r="R27" s="44"/>
       <c r="S27" s="44"/>
-      <c r="T27" s="66"/>
-      <c r="U27" s="67"/>
-      <c r="V27" s="67"/>
-      <c r="W27" s="67"/>
-      <c r="X27" s="67"/>
-      <c r="Y27" s="67"/>
-      <c r="Z27" s="67"/>
-      <c r="AA27" s="68"/>
+      <c r="T27" s="77"/>
+      <c r="U27" s="78"/>
+      <c r="V27" s="78"/>
+      <c r="W27" s="78"/>
+      <c r="X27" s="78"/>
+      <c r="Y27" s="78"/>
+      <c r="Z27" s="78"/>
+      <c r="AA27" s="79"/>
       <c r="AB27" s="44"/>
       <c r="AC27" s="44"/>
       <c r="AD27" s="44"/>
@@ -4363,9 +4372,9 @@
       <c r="CC27" s="44"/>
       <c r="CD27" s="44"/>
       <c r="CE27" s="44"/>
-      <c r="CF27" s="60"/>
+      <c r="CF27" s="71"/>
     </row>
-    <row r="28" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
         <v>56</v>
       </c>
@@ -4387,14 +4396,14 @@
       <c r="Q28" s="44"/>
       <c r="R28" s="44"/>
       <c r="S28" s="44"/>
-      <c r="T28" s="66"/>
-      <c r="U28" s="67"/>
-      <c r="V28" s="67"/>
-      <c r="W28" s="67"/>
-      <c r="X28" s="67"/>
-      <c r="Y28" s="67"/>
-      <c r="Z28" s="67"/>
-      <c r="AA28" s="68"/>
+      <c r="T28" s="77"/>
+      <c r="U28" s="78"/>
+      <c r="V28" s="78"/>
+      <c r="W28" s="78"/>
+      <c r="X28" s="78"/>
+      <c r="Y28" s="78"/>
+      <c r="Z28" s="78"/>
+      <c r="AA28" s="79"/>
       <c r="AB28" s="44"/>
       <c r="AC28" s="44"/>
       <c r="AD28" s="44"/>
@@ -4463,9 +4472,9 @@
       <c r="CC28" s="44"/>
       <c r="CD28" s="44"/>
       <c r="CE28" s="44"/>
-      <c r="CF28" s="60"/>
+      <c r="CF28" s="71"/>
     </row>
-    <row r="29" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
         <v>60</v>
       </c>
@@ -4487,14 +4496,14 @@
       <c r="Q29" s="44"/>
       <c r="R29" s="44"/>
       <c r="S29" s="44"/>
-      <c r="T29" s="66"/>
-      <c r="U29" s="67"/>
-      <c r="V29" s="67"/>
-      <c r="W29" s="67"/>
-      <c r="X29" s="67"/>
-      <c r="Y29" s="67"/>
-      <c r="Z29" s="67"/>
-      <c r="AA29" s="68"/>
+      <c r="T29" s="77"/>
+      <c r="U29" s="78"/>
+      <c r="V29" s="78"/>
+      <c r="W29" s="78"/>
+      <c r="X29" s="78"/>
+      <c r="Y29" s="78"/>
+      <c r="Z29" s="78"/>
+      <c r="AA29" s="79"/>
       <c r="AB29" s="44"/>
       <c r="AC29" s="44"/>
       <c r="AD29" s="44"/>
@@ -4536,8 +4545,12 @@
       <c r="AX29" s="44"/>
       <c r="AY29" s="44"/>
       <c r="AZ29" s="44"/>
-      <c r="BA29" s="45"/>
-      <c r="BB29" s="45"/>
+      <c r="BA29" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB29" s="45" t="s">
+        <v>57</v>
+      </c>
       <c r="BC29" s="44"/>
       <c r="BD29" s="44"/>
       <c r="BE29" s="44"/>
@@ -4567,10 +4580,10 @@
       <c r="CC29" s="44"/>
       <c r="CD29" s="44"/>
       <c r="CE29" s="44"/>
-      <c r="CF29" s="60"/>
+      <c r="CF29" s="71"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A30" s="84" t="s">
+    <row r="30" spans="1:84" ht="13" x14ac:dyDescent="0.3">
+      <c r="A30" s="42" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="16"/>
@@ -4591,14 +4604,14 @@
       <c r="Q30" s="44"/>
       <c r="R30" s="44"/>
       <c r="S30" s="44"/>
-      <c r="T30" s="66"/>
-      <c r="U30" s="67"/>
-      <c r="V30" s="67"/>
-      <c r="W30" s="67"/>
-      <c r="X30" s="67"/>
-      <c r="Y30" s="67"/>
-      <c r="Z30" s="67"/>
-      <c r="AA30" s="68"/>
+      <c r="T30" s="77"/>
+      <c r="U30" s="78"/>
+      <c r="V30" s="78"/>
+      <c r="W30" s="78"/>
+      <c r="X30" s="78"/>
+      <c r="Y30" s="78"/>
+      <c r="Z30" s="78"/>
+      <c r="AA30" s="79"/>
       <c r="AB30" s="44"/>
       <c r="AC30" s="44"/>
       <c r="AD30" s="44"/>
@@ -4626,15 +4639,33 @@
       <c r="AZ30" s="44"/>
       <c r="BA30" s="44"/>
       <c r="BB30" s="44"/>
-      <c r="BC30" s="45"/>
-      <c r="BD30" s="45"/>
-      <c r="BE30" s="45"/>
-      <c r="BF30" s="45"/>
-      <c r="BG30" s="45"/>
-      <c r="BH30" s="44"/>
-      <c r="BI30" s="44"/>
-      <c r="BJ30" s="44"/>
-      <c r="BK30" s="44"/>
+      <c r="BC30" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="BD30" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE30" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF30" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG30" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH30" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI30" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ30" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="BK30" s="44" t="s">
+        <v>57</v>
+      </c>
       <c r="BL30" s="44"/>
       <c r="BM30" s="44"/>
       <c r="BN30" s="44"/>
@@ -4655,10 +4686,10 @@
       <c r="CC30" s="44"/>
       <c r="CD30" s="44"/>
       <c r="CE30" s="44"/>
-      <c r="CF30" s="60"/>
+      <c r="CF30" s="71"/>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A31" s="84" t="s">
+    <row r="31" spans="1:84" ht="13" x14ac:dyDescent="0.3">
+      <c r="A31" s="42" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="16"/>
@@ -4679,14 +4710,14 @@
       <c r="Q31" s="44"/>
       <c r="R31" s="44"/>
       <c r="S31" s="44"/>
-      <c r="T31" s="66"/>
-      <c r="U31" s="67"/>
-      <c r="V31" s="67"/>
-      <c r="W31" s="67"/>
-      <c r="X31" s="67"/>
-      <c r="Y31" s="67"/>
-      <c r="Z31" s="67"/>
-      <c r="AA31" s="68"/>
+      <c r="T31" s="77"/>
+      <c r="U31" s="78"/>
+      <c r="V31" s="78"/>
+      <c r="W31" s="78"/>
+      <c r="X31" s="78"/>
+      <c r="Y31" s="78"/>
+      <c r="Z31" s="78"/>
+      <c r="AA31" s="79"/>
       <c r="AB31" s="44"/>
       <c r="AC31" s="44"/>
       <c r="AD31" s="44"/>
@@ -4716,9 +4747,15 @@
       <c r="BB31" s="44"/>
       <c r="BC31" s="44"/>
       <c r="BD31" s="44"/>
-      <c r="BE31" s="46"/>
-      <c r="BF31" s="46"/>
-      <c r="BG31" s="46"/>
+      <c r="BE31" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BF31" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BG31" s="46" t="s">
+        <v>41</v>
+      </c>
       <c r="BH31" s="44"/>
       <c r="BI31" s="44"/>
       <c r="BJ31" s="44"/>
@@ -4743,9 +4780,9 @@
       <c r="CC31" s="44"/>
       <c r="CD31" s="44"/>
       <c r="CE31" s="44"/>
-      <c r="CF31" s="60"/>
+      <c r="CF31" s="71"/>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="42" t="s">
         <v>53</v>
       </c>
@@ -4767,14 +4804,14 @@
       <c r="Q32" s="44"/>
       <c r="R32" s="44"/>
       <c r="S32" s="44"/>
-      <c r="T32" s="66"/>
-      <c r="U32" s="67"/>
-      <c r="V32" s="67"/>
-      <c r="W32" s="67"/>
-      <c r="X32" s="67"/>
-      <c r="Y32" s="67"/>
-      <c r="Z32" s="67"/>
-      <c r="AA32" s="68"/>
+      <c r="T32" s="77"/>
+      <c r="U32" s="78"/>
+      <c r="V32" s="78"/>
+      <c r="W32" s="78"/>
+      <c r="X32" s="78"/>
+      <c r="Y32" s="78"/>
+      <c r="Z32" s="78"/>
+      <c r="AA32" s="79"/>
       <c r="AB32" s="44"/>
       <c r="AC32" s="44"/>
       <c r="AD32" s="44"/>
@@ -4800,10 +4837,18 @@
       <c r="AX32" s="44"/>
       <c r="AY32" s="44"/>
       <c r="AZ32" s="44"/>
-      <c r="BA32" s="46"/>
-      <c r="BB32" s="46"/>
-      <c r="BC32" s="46"/>
-      <c r="BD32" s="46"/>
+      <c r="BA32" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB32" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC32" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="BD32" s="46" t="s">
+        <v>41</v>
+      </c>
       <c r="BE32" s="3"/>
       <c r="BF32" s="44"/>
       <c r="BG32" s="44"/>
@@ -4831,9 +4876,9 @@
       <c r="CC32" s="44"/>
       <c r="CD32" s="44"/>
       <c r="CE32" s="44"/>
-      <c r="CF32" s="60"/>
+      <c r="CF32" s="71"/>
     </row>
-    <row r="33" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
         <v>55</v>
       </c>
@@ -4855,14 +4900,14 @@
       <c r="Q33" s="44"/>
       <c r="R33" s="44"/>
       <c r="S33" s="44"/>
-      <c r="T33" s="66"/>
-      <c r="U33" s="67"/>
-      <c r="V33" s="67"/>
-      <c r="W33" s="67"/>
-      <c r="X33" s="67"/>
-      <c r="Y33" s="67"/>
-      <c r="Z33" s="67"/>
-      <c r="AA33" s="68"/>
+      <c r="T33" s="77"/>
+      <c r="U33" s="78"/>
+      <c r="V33" s="78"/>
+      <c r="W33" s="78"/>
+      <c r="X33" s="78"/>
+      <c r="Y33" s="78"/>
+      <c r="Z33" s="78"/>
+      <c r="AA33" s="79"/>
       <c r="AB33" s="44"/>
       <c r="AC33" s="44"/>
       <c r="AD33" s="44"/>
@@ -4919,9 +4964,9 @@
       <c r="CC33" s="44"/>
       <c r="CD33" s="44"/>
       <c r="CE33" s="44"/>
-      <c r="CF33" s="60"/>
+      <c r="CF33" s="71"/>
     </row>
-    <row r="34" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
         <v>21</v>
       </c>
@@ -4945,14 +4990,14 @@
       <c r="Q34" s="44"/>
       <c r="R34" s="44"/>
       <c r="S34" s="44"/>
-      <c r="T34" s="66"/>
-      <c r="U34" s="67"/>
-      <c r="V34" s="67"/>
-      <c r="W34" s="67"/>
-      <c r="X34" s="67"/>
-      <c r="Y34" s="67"/>
-      <c r="Z34" s="67"/>
-      <c r="AA34" s="68"/>
+      <c r="T34" s="77"/>
+      <c r="U34" s="78"/>
+      <c r="V34" s="78"/>
+      <c r="W34" s="78"/>
+      <c r="X34" s="78"/>
+      <c r="Y34" s="78"/>
+      <c r="Z34" s="78"/>
+      <c r="AA34" s="79"/>
       <c r="AB34" s="44"/>
       <c r="AC34" s="44"/>
       <c r="AD34" s="44"/>
@@ -5009,9 +5054,9 @@
       <c r="CC34" s="44"/>
       <c r="CD34" s="44"/>
       <c r="CE34" s="44"/>
-      <c r="CF34" s="60"/>
+      <c r="CF34" s="71"/>
     </row>
-    <row r="35" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>22</v>
       </c>
@@ -5043,14 +5088,14 @@
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
       <c r="S35" s="44"/>
-      <c r="T35" s="66"/>
-      <c r="U35" s="67"/>
-      <c r="V35" s="67"/>
-      <c r="W35" s="67"/>
-      <c r="X35" s="67"/>
-      <c r="Y35" s="67"/>
-      <c r="Z35" s="67"/>
-      <c r="AA35" s="68"/>
+      <c r="T35" s="77"/>
+      <c r="U35" s="78"/>
+      <c r="V35" s="78"/>
+      <c r="W35" s="78"/>
+      <c r="X35" s="78"/>
+      <c r="Y35" s="78"/>
+      <c r="Z35" s="78"/>
+      <c r="AA35" s="79"/>
       <c r="AB35" s="44"/>
       <c r="AC35" s="44"/>
       <c r="AD35" s="44"/>
@@ -5107,9 +5152,9 @@
       <c r="CC35" s="44"/>
       <c r="CD35" s="44"/>
       <c r="CE35" s="44"/>
-      <c r="CF35" s="60"/>
+      <c r="CF35" s="71"/>
     </row>
-    <row r="36" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>23</v>
       </c>
@@ -5141,14 +5186,14 @@
       <c r="Q36" s="44"/>
       <c r="R36" s="44"/>
       <c r="S36" s="44"/>
-      <c r="T36" s="66"/>
-      <c r="U36" s="67"/>
-      <c r="V36" s="67"/>
-      <c r="W36" s="67"/>
-      <c r="X36" s="67"/>
-      <c r="Y36" s="67"/>
-      <c r="Z36" s="67"/>
-      <c r="AA36" s="68"/>
+      <c r="T36" s="77"/>
+      <c r="U36" s="78"/>
+      <c r="V36" s="78"/>
+      <c r="W36" s="78"/>
+      <c r="X36" s="78"/>
+      <c r="Y36" s="78"/>
+      <c r="Z36" s="78"/>
+      <c r="AA36" s="79"/>
       <c r="AB36" s="44"/>
       <c r="AC36" s="44"/>
       <c r="AD36" s="44"/>
@@ -5205,9 +5250,9 @@
       <c r="CC36" s="44"/>
       <c r="CD36" s="44"/>
       <c r="CE36" s="44"/>
-      <c r="CF36" s="60"/>
+      <c r="CF36" s="71"/>
     </row>
-    <row r="37" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
         <v>24</v>
       </c>
@@ -5239,14 +5284,14 @@
       <c r="Q37" s="44"/>
       <c r="R37" s="44"/>
       <c r="S37" s="44"/>
-      <c r="T37" s="66"/>
-      <c r="U37" s="67"/>
-      <c r="V37" s="67"/>
-      <c r="W37" s="67"/>
-      <c r="X37" s="67"/>
-      <c r="Y37" s="67"/>
-      <c r="Z37" s="67"/>
-      <c r="AA37" s="68"/>
+      <c r="T37" s="77"/>
+      <c r="U37" s="78"/>
+      <c r="V37" s="78"/>
+      <c r="W37" s="78"/>
+      <c r="X37" s="78"/>
+      <c r="Y37" s="78"/>
+      <c r="Z37" s="78"/>
+      <c r="AA37" s="79"/>
       <c r="AB37" s="46" t="s">
         <v>39</v>
       </c>
@@ -5307,9 +5352,9 @@
       <c r="CC37" s="44"/>
       <c r="CD37" s="44"/>
       <c r="CE37" s="44"/>
-      <c r="CF37" s="60"/>
+      <c r="CF37" s="71"/>
     </row>
-    <row r="38" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>25</v>
       </c>
@@ -5333,14 +5378,14 @@
       <c r="Q38" s="44"/>
       <c r="R38" s="44"/>
       <c r="S38" s="44"/>
-      <c r="T38" s="66"/>
-      <c r="U38" s="67"/>
-      <c r="V38" s="67"/>
-      <c r="W38" s="67"/>
-      <c r="X38" s="67"/>
-      <c r="Y38" s="67"/>
-      <c r="Z38" s="67"/>
-      <c r="AA38" s="68"/>
+      <c r="T38" s="77"/>
+      <c r="U38" s="78"/>
+      <c r="V38" s="78"/>
+      <c r="W38" s="78"/>
+      <c r="X38" s="78"/>
+      <c r="Y38" s="78"/>
+      <c r="Z38" s="78"/>
+      <c r="AA38" s="79"/>
       <c r="AB38" s="47"/>
       <c r="AC38" s="44"/>
       <c r="AD38" s="44"/>
@@ -5397,9 +5442,9 @@
       <c r="CC38" s="44"/>
       <c r="CD38" s="44"/>
       <c r="CE38" s="44"/>
-      <c r="CF38" s="60"/>
+      <c r="CF38" s="71"/>
     </row>
-    <row r="39" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
         <v>26</v>
       </c>
@@ -5423,14 +5468,14 @@
       <c r="Q39" s="44"/>
       <c r="R39" s="44"/>
       <c r="S39" s="44"/>
-      <c r="T39" s="66"/>
-      <c r="U39" s="67"/>
-      <c r="V39" s="67"/>
-      <c r="W39" s="67"/>
-      <c r="X39" s="67"/>
-      <c r="Y39" s="67"/>
-      <c r="Z39" s="67"/>
-      <c r="AA39" s="68"/>
+      <c r="T39" s="77"/>
+      <c r="U39" s="78"/>
+      <c r="V39" s="78"/>
+      <c r="W39" s="78"/>
+      <c r="X39" s="78"/>
+      <c r="Y39" s="78"/>
+      <c r="Z39" s="78"/>
+      <c r="AA39" s="79"/>
       <c r="AB39" s="44"/>
       <c r="AC39" s="44"/>
       <c r="AD39" s="46" t="s">
@@ -5459,10 +5504,18 @@
       <c r="AW39" s="44"/>
       <c r="AX39" s="44"/>
       <c r="AY39" s="44"/>
-      <c r="AZ39" s="49"/>
-      <c r="BA39" s="49"/>
-      <c r="BB39" s="49"/>
-      <c r="BC39" s="49"/>
+      <c r="AZ39" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="BA39" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="BB39" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="BC39" s="49" t="s">
+        <v>40</v>
+      </c>
       <c r="BD39" s="44"/>
       <c r="BE39" s="44"/>
       <c r="BF39" s="44"/>
@@ -5491,9 +5544,9 @@
       <c r="CC39" s="44"/>
       <c r="CD39" s="44"/>
       <c r="CE39" s="44"/>
-      <c r="CF39" s="60"/>
+      <c r="CF39" s="71"/>
     </row>
-    <row r="40" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
         <v>27</v>
       </c>
@@ -5541,14 +5594,14 @@
       <c r="Q40" s="44"/>
       <c r="R40" s="44"/>
       <c r="S40" s="44"/>
-      <c r="T40" s="66"/>
-      <c r="U40" s="67"/>
-      <c r="V40" s="67"/>
-      <c r="W40" s="67"/>
-      <c r="X40" s="67"/>
-      <c r="Y40" s="67"/>
-      <c r="Z40" s="67"/>
-      <c r="AA40" s="68"/>
+      <c r="T40" s="77"/>
+      <c r="U40" s="78"/>
+      <c r="V40" s="78"/>
+      <c r="W40" s="78"/>
+      <c r="X40" s="78"/>
+      <c r="Y40" s="78"/>
+      <c r="Z40" s="78"/>
+      <c r="AA40" s="79"/>
       <c r="AB40" s="50" t="s">
         <v>39</v>
       </c>
@@ -5589,10 +5642,18 @@
       <c r="BE40" s="50"/>
       <c r="BF40" s="50"/>
       <c r="BG40" s="50"/>
-      <c r="BH40" s="50"/>
-      <c r="BI40" s="50"/>
-      <c r="BJ40" s="50"/>
-      <c r="BK40" s="50"/>
+      <c r="BH40" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="BI40" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="BJ40" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK40" s="50" t="s">
+        <v>40</v>
+      </c>
       <c r="BL40" s="44"/>
       <c r="BM40" s="44"/>
       <c r="BN40" s="44"/>
@@ -5613,9 +5674,9 @@
       <c r="CC40" s="44"/>
       <c r="CD40" s="44"/>
       <c r="CE40" s="44"/>
-      <c r="CF40" s="60"/>
+      <c r="CF40" s="71"/>
     </row>
-    <row r="41" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
         <v>28</v>
       </c>
@@ -5639,14 +5700,14 @@
       <c r="Q41" s="44"/>
       <c r="R41" s="44"/>
       <c r="S41" s="44"/>
-      <c r="T41" s="66"/>
-      <c r="U41" s="67"/>
-      <c r="V41" s="67"/>
-      <c r="W41" s="67"/>
-      <c r="X41" s="67"/>
-      <c r="Y41" s="67"/>
-      <c r="Z41" s="67"/>
-      <c r="AA41" s="68"/>
+      <c r="T41" s="77"/>
+      <c r="U41" s="78"/>
+      <c r="V41" s="78"/>
+      <c r="W41" s="78"/>
+      <c r="X41" s="78"/>
+      <c r="Y41" s="78"/>
+      <c r="Z41" s="78"/>
+      <c r="AA41" s="79"/>
       <c r="AB41" s="44"/>
       <c r="AC41" s="3"/>
       <c r="AD41" s="34"/>
@@ -5705,9 +5766,9 @@
       <c r="CC41" s="44"/>
       <c r="CD41" s="44"/>
       <c r="CE41" s="44"/>
-      <c r="CF41" s="60"/>
+      <c r="CF41" s="71"/>
     </row>
-    <row r="42" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:84" ht="13" x14ac:dyDescent="0.3">
       <c r="A42" s="40" t="s">
         <v>32</v>
       </c>
@@ -5729,14 +5790,14 @@
       <c r="Q42" s="44"/>
       <c r="R42" s="44"/>
       <c r="S42" s="44"/>
-      <c r="T42" s="66"/>
-      <c r="U42" s="67"/>
-      <c r="V42" s="67"/>
-      <c r="W42" s="67"/>
-      <c r="X42" s="67"/>
-      <c r="Y42" s="67"/>
-      <c r="Z42" s="67"/>
-      <c r="AA42" s="68"/>
+      <c r="T42" s="77"/>
+      <c r="U42" s="78"/>
+      <c r="V42" s="78"/>
+      <c r="W42" s="78"/>
+      <c r="X42" s="78"/>
+      <c r="Y42" s="78"/>
+      <c r="Z42" s="78"/>
+      <c r="AA42" s="79"/>
       <c r="AB42" s="44"/>
       <c r="AC42" s="44"/>
       <c r="AD42" s="44"/>
@@ -5793,9 +5854,9 @@
       <c r="CC42" s="44"/>
       <c r="CD42" s="44"/>
       <c r="CE42" s="44"/>
-      <c r="CF42" s="60"/>
+      <c r="CF42" s="71"/>
     </row>
-    <row r="43" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>33</v>
       </c>
@@ -5817,14 +5878,14 @@
       <c r="Q43" s="44"/>
       <c r="R43" s="44"/>
       <c r="S43" s="44"/>
-      <c r="T43" s="66"/>
-      <c r="U43" s="67"/>
-      <c r="V43" s="67"/>
-      <c r="W43" s="67"/>
-      <c r="X43" s="67"/>
-      <c r="Y43" s="67"/>
-      <c r="Z43" s="67"/>
-      <c r="AA43" s="68"/>
+      <c r="T43" s="77"/>
+      <c r="U43" s="78"/>
+      <c r="V43" s="78"/>
+      <c r="W43" s="78"/>
+      <c r="X43" s="78"/>
+      <c r="Y43" s="78"/>
+      <c r="Z43" s="78"/>
+      <c r="AA43" s="79"/>
       <c r="AB43" s="44"/>
       <c r="AC43" s="44"/>
       <c r="AD43" s="44"/>
@@ -5881,9 +5942,9 @@
       <c r="CC43" s="44"/>
       <c r="CD43" s="44"/>
       <c r="CE43" s="44"/>
-      <c r="CF43" s="60"/>
+      <c r="CF43" s="71"/>
     </row>
-    <row r="44" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:84" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="17"/>
       <c r="C44" s="11"/>
@@ -5903,14 +5964,14 @@
       <c r="Q44" s="44"/>
       <c r="R44" s="44"/>
       <c r="S44" s="44"/>
-      <c r="T44" s="69"/>
-      <c r="U44" s="70"/>
-      <c r="V44" s="70"/>
-      <c r="W44" s="70"/>
-      <c r="X44" s="70"/>
-      <c r="Y44" s="70"/>
-      <c r="Z44" s="70"/>
-      <c r="AA44" s="71"/>
+      <c r="T44" s="80"/>
+      <c r="U44" s="81"/>
+      <c r="V44" s="81"/>
+      <c r="W44" s="81"/>
+      <c r="X44" s="81"/>
+      <c r="Y44" s="81"/>
+      <c r="Z44" s="81"/>
+      <c r="AA44" s="82"/>
       <c r="AB44" s="12"/>
       <c r="AC44" s="13"/>
       <c r="AD44" s="13"/>
@@ -5967,105 +6028,109 @@
       <c r="CC44" s="13"/>
       <c r="CD44" s="13"/>
       <c r="CE44" s="14"/>
-      <c r="CF44" s="60"/>
+      <c r="CF44" s="71"/>
     </row>
-    <row r="45" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A45" s="59" t="s">
+    <row r="45" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A45" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="59"/>
-      <c r="L45" s="59"/>
-      <c r="M45" s="59"/>
-      <c r="N45" s="59"/>
-      <c r="O45" s="59"/>
-      <c r="P45" s="59"/>
-      <c r="Q45" s="59"/>
-      <c r="R45" s="59"/>
-      <c r="S45" s="59"/>
-      <c r="T45" s="59"/>
-      <c r="U45" s="59"/>
-      <c r="V45" s="59"/>
-      <c r="W45" s="59"/>
-      <c r="X45" s="59"/>
-      <c r="Y45" s="59"/>
-      <c r="Z45" s="59"/>
-      <c r="AA45" s="59"/>
-      <c r="AB45" s="59"/>
-      <c r="AC45" s="59"/>
-      <c r="AD45" s="59"/>
-      <c r="AE45" s="59"/>
-      <c r="AF45" s="59"/>
-      <c r="AG45" s="59"/>
-      <c r="AH45" s="59"/>
-      <c r="AI45" s="59"/>
-      <c r="AJ45" s="59"/>
-      <c r="AK45" s="59"/>
-      <c r="AL45" s="59"/>
-      <c r="AM45" s="59"/>
-      <c r="AN45" s="59"/>
-      <c r="AO45" s="59"/>
-      <c r="AP45" s="59"/>
-      <c r="AQ45" s="59"/>
-      <c r="AR45" s="59"/>
-      <c r="AS45" s="59"/>
-      <c r="AT45" s="59"/>
-      <c r="AU45" s="59"/>
-      <c r="AV45" s="59"/>
-      <c r="AW45" s="59"/>
-      <c r="AX45" s="59"/>
-      <c r="AY45" s="59"/>
-      <c r="AZ45" s="59"/>
-      <c r="BA45" s="59"/>
-      <c r="BB45" s="59"/>
-      <c r="BC45" s="59"/>
-      <c r="BD45" s="59"/>
-      <c r="BE45" s="59"/>
-      <c r="BF45" s="59"/>
-      <c r="BG45" s="59"/>
-      <c r="BH45" s="59"/>
-      <c r="BI45" s="59"/>
-      <c r="BJ45" s="59"/>
-      <c r="BK45" s="59"/>
-      <c r="BL45" s="59"/>
-      <c r="BM45" s="59"/>
-      <c r="BN45" s="59"/>
-      <c r="BO45" s="59"/>
-      <c r="BP45" s="59"/>
-      <c r="BQ45" s="59"/>
-      <c r="BR45" s="59"/>
-      <c r="BS45" s="59"/>
-      <c r="BT45" s="59"/>
-      <c r="BU45" s="59"/>
-      <c r="BV45" s="59"/>
-      <c r="BW45" s="59"/>
-      <c r="BX45" s="59"/>
-      <c r="BY45" s="59"/>
-      <c r="BZ45" s="59"/>
-      <c r="CA45" s="59"/>
-      <c r="CB45" s="59"/>
-      <c r="CC45" s="59"/>
-      <c r="CD45" s="59"/>
-      <c r="CE45" s="59"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="70"/>
+      <c r="K45" s="70"/>
+      <c r="L45" s="70"/>
+      <c r="M45" s="70"/>
+      <c r="N45" s="70"/>
+      <c r="O45" s="70"/>
+      <c r="P45" s="70"/>
+      <c r="Q45" s="70"/>
+      <c r="R45" s="70"/>
+      <c r="S45" s="70"/>
+      <c r="T45" s="70"/>
+      <c r="U45" s="70"/>
+      <c r="V45" s="70"/>
+      <c r="W45" s="70"/>
+      <c r="X45" s="70"/>
+      <c r="Y45" s="70"/>
+      <c r="Z45" s="70"/>
+      <c r="AA45" s="70"/>
+      <c r="AB45" s="70"/>
+      <c r="AC45" s="70"/>
+      <c r="AD45" s="70"/>
+      <c r="AE45" s="70"/>
+      <c r="AF45" s="70"/>
+      <c r="AG45" s="70"/>
+      <c r="AH45" s="70"/>
+      <c r="AI45" s="70"/>
+      <c r="AJ45" s="70"/>
+      <c r="AK45" s="70"/>
+      <c r="AL45" s="70"/>
+      <c r="AM45" s="70"/>
+      <c r="AN45" s="70"/>
+      <c r="AO45" s="70"/>
+      <c r="AP45" s="70"/>
+      <c r="AQ45" s="70"/>
+      <c r="AR45" s="70"/>
+      <c r="AS45" s="70"/>
+      <c r="AT45" s="70"/>
+      <c r="AU45" s="70"/>
+      <c r="AV45" s="70"/>
+      <c r="AW45" s="70"/>
+      <c r="AX45" s="70"/>
+      <c r="AY45" s="70"/>
+      <c r="AZ45" s="70"/>
+      <c r="BA45" s="70"/>
+      <c r="BB45" s="70"/>
+      <c r="BC45" s="70"/>
+      <c r="BD45" s="70"/>
+      <c r="BE45" s="70"/>
+      <c r="BF45" s="70"/>
+      <c r="BG45" s="70"/>
+      <c r="BH45" s="70"/>
+      <c r="BI45" s="70"/>
+      <c r="BJ45" s="70"/>
+      <c r="BK45" s="70"/>
+      <c r="BL45" s="70"/>
+      <c r="BM45" s="70"/>
+      <c r="BN45" s="70"/>
+      <c r="BO45" s="70"/>
+      <c r="BP45" s="70"/>
+      <c r="BQ45" s="70"/>
+      <c r="BR45" s="70"/>
+      <c r="BS45" s="70"/>
+      <c r="BT45" s="70"/>
+      <c r="BU45" s="70"/>
+      <c r="BV45" s="70"/>
+      <c r="BW45" s="70"/>
+      <c r="BX45" s="70"/>
+      <c r="BY45" s="70"/>
+      <c r="BZ45" s="70"/>
+      <c r="CA45" s="70"/>
+      <c r="CB45" s="70"/>
+      <c r="CC45" s="70"/>
+      <c r="CD45" s="70"/>
+      <c r="CE45" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="X7:AA7"/>
-    <mergeCell ref="D5:AQ6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A45:CE45"/>
+    <mergeCell ref="CF7:CF44"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="T9:AA44"/>
+    <mergeCell ref="AZ7:BC7"/>
+    <mergeCell ref="BD7:BG7"/>
+    <mergeCell ref="BH7:BK7"/>
+    <mergeCell ref="BL7:BO7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="AR5:CE6"/>
     <mergeCell ref="AJ7:AM7"/>
     <mergeCell ref="AN7:AQ7"/>
@@ -6080,18 +6145,14 @@
     <mergeCell ref="BP7:BS7"/>
     <mergeCell ref="BX7:CA7"/>
     <mergeCell ref="CB7:CE7"/>
-    <mergeCell ref="A45:CE45"/>
-    <mergeCell ref="CF7:CF44"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="T9:AA44"/>
-    <mergeCell ref="AZ7:BC7"/>
-    <mergeCell ref="BD7:BG7"/>
-    <mergeCell ref="BH7:BK7"/>
-    <mergeCell ref="BL7:BO7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="X7:AA7"/>
+    <mergeCell ref="D5:AQ6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="B9:B44">
@@ -6333,15 +6394,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
@@ -6350,6 +6402,15 @@
     <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6372,14 +6433,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2702F0-3EB0-496B-8166-A9BB237AECA6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -6394,4 +6447,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>